<commit_message>
Added updated Excel Template - EFCT
Added updated Excel Template - EFCT
</commit_message>
<xml_diff>
--- a/Excel Template - EFCT.xlsx
+++ b/Excel Template - EFCT.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rameel.sher.khan\Documents\EFCT\EFCT UAT\Entity Field Creation Tool - UAT - v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EFCT\EFCT\EFCT Excel Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A96D5DA-FB44-42E3-82DC-884360D77403}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3EFFE1-2CC1-43A4-A47B-CA0D821A93CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="B/ySx6NytDqMnX0W9c+9+oa8uxmimfr8s0HTk/N4vAdswDBVPBFDgISCiviK9IBNlM9s8W+qql9ly5vr6Jy62w==" workbookSaltValue="ZZD3/aUpzVYjJNBgCzhBtA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="828" xr2:uid="{5257C586-A7FD-42E1-B334-B57D3FAB3BE9}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" tabRatio="828" xr2:uid="{5257C586-A7FD-42E1-B334-B57D3FAB3BE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Field - Single Line of Text" sheetId="5" r:id="rId1"/>
@@ -654,7 +655,7 @@
       <formula1>-100000000000</formula1>
       <formula2>100000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hint ::" prompt="Default Format will be 0." sqref="D2:D1048576" xr:uid="{E619EDC3-67B2-4D74-9DCA-5B84ABFB1C2D}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter whole number value from 0 to 10" promptTitle="Hint ::" prompt="Enter value from 0 to 10._x000a_Default Precision will be 2." sqref="D2:D1048576" xr:uid="{E619EDC3-67B2-4D74-9DCA-5B84ABFB1C2D}">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
@@ -716,7 +717,7 @@
       <formula1>-100000000000</formula1>
       <formula2>100000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hint ::" prompt="Default Format will be 0." sqref="D2:D1048576" xr:uid="{5D09F9FA-175C-4051-8E49-84E5A350ED53}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Enter value from 0 to 5" promptTitle="Hint ::" prompt="Enter value from 0 to 5._x000a_Default Precision will be 2." sqref="D2:D1048576" xr:uid="{5D09F9FA-175C-4051-8E49-84E5A350ED53}">
       <formula1>0</formula1>
       <formula2>5</formula2>
     </dataValidation>
@@ -940,7 +941,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hint ::" prompt="Default type will be Look Up." sqref="D2:D1048576" xr:uid="{1F91FD38-C326-4E60-B75B-F2220AF25ABA}">
       <formula1>"Look Up,Customer"</formula1>
     </dataValidation>
@@ -948,6 +949,7 @@
       <formula1>"Optional, Business Required, Business Recommended"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hint ::" prompt="If left empty, default will be System Calculated Schema Name as per Display Name" sqref="B2:B1048576" xr:uid="{3A40D4E4-8321-44B6-BD54-D8651C143EB2}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This column can be left empty for fields of type Customer" sqref="E2:E1048576" xr:uid="{0F2DC67A-1BDB-4A4B-B63D-85BEFBA89CB7}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>